<commit_message>
weekly average sentiment for all companies added
</commit_message>
<xml_diff>
--- a/data/apple/sentiment/apple_averages.xlsx
+++ b/data/apple/sentiment/apple_averages.xlsx
@@ -908,21 +908,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J1" sqref="J1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" customWidth="1"/>
+    <col min="3" max="3" width="5.36328125" customWidth="1"/>
+    <col min="4" max="4" width="5.81640625" customWidth="1"/>
+    <col min="5" max="5" width="6" customWidth="1"/>
+    <col min="6" max="6" width="6.7265625" customWidth="1"/>
+    <col min="7" max="7" width="6.1796875" customWidth="1"/>
+    <col min="8" max="8" width="5.7265625" customWidth="1"/>
+    <col min="9" max="9" width="5.26953125" customWidth="1"/>
+    <col min="10" max="10" width="5.36328125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="4.81640625" customWidth="1"/>
+    <col min="12" max="12" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
@@ -4473,7 +4476,7 @@
         <v>-0.18530232923721351</v>
       </c>
       <c r="D101">
-        <f t="shared" ref="D101:D132" si="22">AVERAGE(B98:B101)</f>
+        <f t="shared" ref="D101:D112" si="22">AVERAGE(B98:B101)</f>
         <v>-0.57861846173134435</v>
       </c>
       <c r="E101">
@@ -4624,7 +4627,7 @@
         <v>-0.50549691967545107</v>
       </c>
       <c r="E105">
-        <f t="shared" ref="E105:E136" si="24">AVERAGE(B98:B105)</f>
+        <f t="shared" ref="E105:E112" si="24">AVERAGE(B98:B105)</f>
         <v>-0.54205769070339771</v>
       </c>
       <c r="F105">

</xml_diff>

<commit_message>
edited all averages and added historical prices
</commit_message>
<xml_diff>
--- a/data/apple/sentiment/apple_averages.xlsx
+++ b/data/apple/sentiment/apple_averages.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldona\Desktop\data_project\fund\data\apple\sentiment\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="24816"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16580" windowHeight="5780"/>
+    <workbookView xWindow="120" yWindow="0" windowWidth="26180" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="apple_averages" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Week</t>
   </si>
@@ -54,12 +54,15 @@
   <si>
     <t>PxCh</t>
   </si>
+  <si>
+    <t>PxCh 1 Week Later</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +193,22 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -498,7 +517,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -542,6 +561,10 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -551,7 +574,7 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="47">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
@@ -580,11 +603,15 @@
     <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
@@ -652,7 +679,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -704,7 +731,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -898,7 +925,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -906,29 +933,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L112"/>
+  <dimension ref="A1:M112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L1"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="5.36328125" customWidth="1"/>
-    <col min="4" max="4" width="5.81640625" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="6.7265625" customWidth="1"/>
-    <col min="7" max="7" width="6.1796875" customWidth="1"/>
-    <col min="8" max="8" width="5.7265625" customWidth="1"/>
-    <col min="9" max="9" width="5.26953125" customWidth="1"/>
-    <col min="10" max="10" width="5.36328125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="4.81640625" customWidth="1"/>
-    <col min="12" max="12" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.83203125" customWidth="1"/>
+    <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -960,14 +988,17 @@
         <v>10</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L1">
+      <c r="M1">
         <f>-0.4889571</f>
         <v>-0.48895709999999998</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <v>42053</v>
       </c>
@@ -975,11 +1006,11 @@
         <v>0.28784253659974801</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:F33" si="0">B2-$L$1</f>
+        <f t="shared" ref="F2:F33" si="0">B2-$M$1</f>
         <v>0.77679963659974804</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>42060</v>
       </c>
@@ -995,11 +1026,11 @@
         <v>-0.23391795654326303</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G34" si="1">C3-$L$1</f>
+        <f t="shared" ref="G3:G34" si="1">C3-$M$1</f>
         <v>0.27144084002824248</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>42067</v>
       </c>
@@ -1019,7 +1050,7 @@
         <v>-8.819806209888309E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13">
       <c r="A5" s="1">
         <v>42074</v>
       </c>
@@ -1043,11 +1074,11 @@
         <v>5.4021393081839453E-2</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H36" si="4">D5-$L$1</f>
+        <f t="shared" ref="H5:H36" si="4">D5-$M$1</f>
         <v>0.16273111655504097</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13">
       <c r="A6" s="1">
         <v>42081</v>
       </c>
@@ -1075,7 +1106,7 @@
         <v>0.20579219498185169</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13">
       <c r="A7" s="1">
         <v>42088</v>
       </c>
@@ -1103,7 +1134,7 @@
         <v>0.66755054473649</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13">
       <c r="A8" s="1">
         <v>42095</v>
       </c>
@@ -1131,7 +1162,7 @@
         <v>0.74153442348090204</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13">
       <c r="A9" s="1">
         <v>42102</v>
       </c>
@@ -1163,11 +1194,11 @@
         <v>1.1194998613268865</v>
       </c>
       <c r="I9">
-        <f t="shared" ref="I9:I40" si="6">E9-$L$1</f>
+        <f t="shared" ref="I9:I40" si="6">E9-$M$1</f>
         <v>0.64111548894096371</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13">
       <c r="A10" s="1">
         <v>42109</v>
       </c>
@@ -1203,7 +1234,7 @@
         <v>0.60384213289377298</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13">
       <c r="A11" s="1">
         <v>42116</v>
       </c>
@@ -1239,7 +1270,7 @@
         <v>0.77276322037565126</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" s="3" customFormat="1">
       <c r="A12" s="2">
         <v>42123</v>
       </c>
@@ -1277,8 +1308,9 @@
       <c r="J12" s="5">
         <v>-1.5800000000000002E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1">
         <v>42130</v>
       </c>
@@ -1314,7 +1346,7 @@
         <v>0.86080413445295867</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13">
       <c r="A14" s="1">
         <v>42137</v>
       </c>
@@ -1350,7 +1382,7 @@
         <v>0.82437761247038832</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13">
       <c r="A15" s="1">
         <v>42144</v>
       </c>
@@ -1386,7 +1418,7 @@
         <v>0.67150087420348969</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13">
       <c r="A16" s="1">
         <v>42151</v>
       </c>
@@ -1422,7 +1454,7 @@
         <v>0.50983224863163912</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11">
       <c r="A17" s="1">
         <v>42158</v>
       </c>
@@ -1458,7 +1490,7 @@
         <v>0.50340965043997032</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11">
       <c r="A18" s="1">
         <v>42165</v>
       </c>
@@ -1494,7 +1526,7 @@
         <v>0.55731620000697613</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11">
       <c r="A19" s="1">
         <v>42172</v>
       </c>
@@ -1530,7 +1562,7 @@
         <v>0.55181268105787784</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11">
       <c r="A20" s="1">
         <v>42179</v>
       </c>
@@ -1566,7 +1598,7 @@
         <v>0.52504924543826537</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11">
       <c r="A21" s="1">
         <v>42186</v>
       </c>
@@ -1602,7 +1634,7 @@
         <v>0.49788366454196953</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11">
       <c r="A22" s="1">
         <v>42193</v>
       </c>
@@ -1638,7 +1670,7 @@
         <v>0.46685268585850648</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11">
       <c r="A23" s="1">
         <v>42200</v>
       </c>
@@ -1674,7 +1706,7 @@
         <v>0.51648175324286283</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" s="3" customFormat="1">
       <c r="A24" s="2">
         <v>42207</v>
       </c>
@@ -1712,8 +1744,9 @@
       <c r="J24" s="5">
         <v>-4.2299999999999997E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:11">
       <c r="A25" s="1">
         <v>42214</v>
       </c>
@@ -1749,7 +1782,7 @@
         <v>0.69470331076020786</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11">
       <c r="A26" s="1">
         <v>42221</v>
       </c>
@@ -1785,7 +1818,7 @@
         <v>0.64168345157250384</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11">
       <c r="A27" s="1">
         <v>42228</v>
       </c>
@@ -1821,7 +1854,7 @@
         <v>0.5883882716882185</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11">
       <c r="A28" s="1">
         <v>42235</v>
       </c>
@@ -1857,7 +1890,7 @@
         <v>0.6402252885550499</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11">
       <c r="A29" s="1">
         <v>42242</v>
       </c>
@@ -1893,7 +1926,7 @@
         <v>0.68039275644410835</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11">
       <c r="A30" s="1">
         <v>42249</v>
       </c>
@@ -1929,7 +1962,7 @@
         <v>0.69226471524291822</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11">
       <c r="A31" s="1">
         <v>42256</v>
       </c>
@@ -1965,7 +1998,7 @@
         <v>0.76065810719601901</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11">
       <c r="A32" s="1">
         <v>42263</v>
       </c>
@@ -2001,7 +2034,7 @@
         <v>0.51393605461584357</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11">
       <c r="A33" s="1">
         <v>42270</v>
       </c>
@@ -2037,7 +2070,7 @@
         <v>0.46080808774364895</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11">
       <c r="A34" s="1">
         <v>42277</v>
       </c>
@@ -2057,7 +2090,7 @@
         <v>2.7067833322201449E-2</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F65" si="7">B34-$L$1</f>
+        <f t="shared" ref="F34:F65" si="7">B34-$M$1</f>
         <v>0.92744107588505698</v>
       </c>
       <c r="G34">
@@ -2073,7 +2106,7 @@
         <v>0.51602493332220145</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11">
       <c r="A35" s="1">
         <v>42284</v>
       </c>
@@ -2097,7 +2130,7 @@
         <v>1.5929446650939498</v>
       </c>
       <c r="G35">
-        <f t="shared" ref="G35:G66" si="8">C35-$L$1</f>
+        <f t="shared" ref="G35:G66" si="8">C35-$M$1</f>
         <v>1.2601928704895033</v>
       </c>
       <c r="H35">
@@ -2109,7 +2142,7 @@
         <v>0.63426037237835842</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11">
       <c r="A36" s="1">
         <v>42291</v>
       </c>
@@ -2145,7 +2178,7 @@
         <v>0.61189099701668614</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11">
       <c r="A37" s="1">
         <v>42298</v>
       </c>
@@ -2173,7 +2206,7 @@
         <v>0.61037397753225342</v>
       </c>
       <c r="H37">
-        <f t="shared" ref="H37:H68" si="10">D37-$L$1</f>
+        <f t="shared" ref="H37:H68" si="10">D37-$M$1</f>
         <v>0.93528342401087849</v>
       </c>
       <c r="I37">
@@ -2181,7 +2214,7 @@
         <v>0.64723213617367292</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" s="3" customFormat="1">
       <c r="A38" s="2">
         <v>42305</v>
       </c>
@@ -2219,8 +2252,9 @@
       <c r="J38" s="5">
         <v>4.1200000000000001E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="1:11">
       <c r="A39" s="1">
         <v>42312</v>
       </c>
@@ -2256,7 +2290,7 @@
         <v>0.64446300071281504</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11">
       <c r="A40" s="1">
         <v>42319</v>
       </c>
@@ -2292,7 +2326,7 @@
         <v>0.91702196049825813</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11">
       <c r="A41" s="1">
         <v>42326</v>
       </c>
@@ -2324,11 +2358,11 @@
         <v>0.75856348383971506</v>
       </c>
       <c r="I41">
-        <f t="shared" ref="I41:I72" si="12">E41-$L$1</f>
+        <f t="shared" ref="I41:I72" si="12">E41-$M$1</f>
         <v>0.84692345392529678</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11">
       <c r="A42" s="1">
         <v>42333</v>
       </c>
@@ -2364,7 +2398,7 @@
         <v>0.86304153503404368</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11">
       <c r="A43" s="1">
         <v>42340</v>
       </c>
@@ -2400,7 +2434,7 @@
         <v>0.76315304075432344</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11">
       <c r="A44" s="1">
         <v>42347</v>
       </c>
@@ -2436,7 +2470,7 @@
         <v>0.88722998766122063</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11">
       <c r="A45" s="1">
         <v>42354</v>
       </c>
@@ -2472,7 +2506,7 @@
         <v>0.82070445693212157</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11">
       <c r="A46" s="1">
         <v>42361</v>
       </c>
@@ -2508,7 +2542,7 @@
         <v>0.70793322739109388</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11">
       <c r="A47" s="1">
         <v>42368</v>
       </c>
@@ -2544,7 +2578,7 @@
         <v>0.56811570370635234</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11">
       <c r="A48" s="1">
         <v>42375</v>
       </c>
@@ -2580,7 +2614,7 @@
         <v>0.41590688638746209</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11">
       <c r="A49" s="1">
         <v>42382</v>
       </c>
@@ -2616,7 +2650,7 @@
         <v>0.48668575954290022</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11">
       <c r="A50" s="1">
         <v>42389</v>
       </c>
@@ -2652,7 +2686,7 @@
         <v>0.41960440443017244</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" s="3" customFormat="1">
       <c r="A51" s="2">
         <v>42396</v>
       </c>
@@ -2690,8 +2724,9 @@
       <c r="J51" s="5">
         <v>-6.5699999999999995E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K51" s="5"/>
+    </row>
+    <row r="52" spans="1:11">
       <c r="A52" s="1">
         <v>42403</v>
       </c>
@@ -2727,7 +2762,7 @@
         <v>0.27589358513447026</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11">
       <c r="A53" s="1">
         <v>42410</v>
       </c>
@@ -2763,7 +2798,7 @@
         <v>0.28948021054110029</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11">
       <c r="A54" s="1">
         <v>42417</v>
       </c>
@@ -2799,7 +2834,7 @@
         <v>-2.0477128345979978E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11">
       <c r="A55" s="1">
         <v>42424</v>
       </c>
@@ -2835,7 +2870,7 @@
         <v>-0.28086002007578897</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11">
       <c r="A56" s="1">
         <v>42431</v>
       </c>
@@ -2871,7 +2906,7 @@
         <v>-0.55357262075096059</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11">
       <c r="A57" s="1">
         <v>42438</v>
       </c>
@@ -2907,7 +2942,7 @@
         <v>-0.75568728647893479</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11">
       <c r="A58" s="1">
         <v>42445</v>
       </c>
@@ -2943,7 +2978,7 @@
         <v>-0.90460692944129861</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11">
       <c r="A59" s="1">
         <v>42452</v>
       </c>
@@ -2979,7 +3014,7 @@
         <v>-1.12183203863787</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11">
       <c r="A60" s="1">
         <v>42459</v>
       </c>
@@ -3015,7 +3050,7 @@
         <v>-1.2763848840155227</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11">
       <c r="A61" s="1">
         <v>42466</v>
       </c>
@@ -3051,7 +3086,7 @@
         <v>-1.4495404193253327</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11">
       <c r="A62" s="1">
         <v>42473</v>
       </c>
@@ -3087,7 +3122,7 @@
         <v>-1.1611876270251174</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11">
       <c r="A63" s="1">
         <v>42480</v>
       </c>
@@ -3123,7 +3158,7 @@
         <v>-0.91448781568188586</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" s="3" customFormat="1">
       <c r="A64" s="2">
         <v>42487</v>
       </c>
@@ -3161,8 +3196,9 @@
       <c r="J64" s="5">
         <v>-6.2600000000000003E-2</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K64" s="5"/>
+    </row>
+    <row r="65" spans="1:11">
       <c r="A65" s="1">
         <v>42494</v>
       </c>
@@ -3198,7 +3234,7 @@
         <v>-0.60691563595176223</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11">
       <c r="A66" s="1">
         <v>42501</v>
       </c>
@@ -3218,7 +3254,7 @@
         <v>-0.9193382081786573</v>
       </c>
       <c r="F66">
-        <f t="shared" ref="F66:F97" si="13">B66-$L$1</f>
+        <f t="shared" ref="F66:F97" si="13">B66-$M$1</f>
         <v>0.74065396233913905</v>
       </c>
       <c r="G66">
@@ -3234,7 +3270,7 @@
         <v>-0.43038110817865732</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11">
       <c r="A67" s="1">
         <v>42508</v>
       </c>
@@ -3258,7 +3294,7 @@
         <v>1.55280649003622</v>
       </c>
       <c r="G67">
-        <f t="shared" ref="G67:G98" si="14">C67-$L$1</f>
+        <f t="shared" ref="G67:G98" si="14">C67-$M$1</f>
         <v>1.1467302261876795</v>
       </c>
       <c r="H67">
@@ -3270,7 +3306,7 @@
         <v>-7.4616224862877389E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11">
       <c r="A68" s="1">
         <v>42515</v>
       </c>
@@ -3306,7 +3342,7 @@
         <v>4.5437729686981454E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11">
       <c r="A69" s="1">
         <v>42522</v>
       </c>
@@ -3334,7 +3370,7 @@
         <v>0.10834529266266896</v>
       </c>
       <c r="H69">
-        <f t="shared" ref="H69:H100" si="17">D69-$L$1</f>
+        <f t="shared" ref="H69:H100" si="17">D69-$M$1</f>
         <v>0.62753775942517431</v>
       </c>
       <c r="I69">
@@ -3342,7 +3378,7 @@
         <v>0.15648921059675863</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11">
       <c r="A70" s="1">
         <v>42529</v>
       </c>
@@ -3378,7 +3414,7 @@
         <v>0.31139258724983315</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11">
       <c r="A71" s="1">
         <v>42536</v>
       </c>
@@ -3414,7 +3450,7 @@
         <v>0.41247493384781986</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11">
       <c r="A72" s="1">
         <v>42543</v>
       </c>
@@ -3450,7 +3486,7 @@
         <v>0.44580067078697883</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11">
       <c r="A73" s="1">
         <v>42550</v>
       </c>
@@ -3482,11 +3518,11 @@
         <v>3.976997029527124E-2</v>
       </c>
       <c r="I73">
-        <f t="shared" ref="I73:I104" si="19">E73-$L$1</f>
+        <f t="shared" ref="I73:I104" si="19">E73-$M$1</f>
         <v>0.33365386486022275</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11">
       <c r="A74" s="1">
         <v>42557</v>
       </c>
@@ -3522,7 +3558,7 @@
         <v>0.35293005816224521</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11">
       <c r="A75" s="1">
         <v>42564</v>
       </c>
@@ -3558,7 +3594,7 @@
         <v>0.24766837866890182</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11">
       <c r="A76" s="1">
         <v>42571</v>
       </c>
@@ -3594,7 +3630,7 @@
         <v>0.27776175316740781</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" s="3" customFormat="1">
       <c r="A77" s="2">
         <v>42578</v>
       </c>
@@ -3632,8 +3668,9 @@
       <c r="J77" s="5">
         <v>6.5000000000000002E-2</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K77" s="5"/>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" s="1">
         <v>42585</v>
       </c>
@@ -3669,7 +3706,7 @@
         <v>0.21837585584559926</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11">
       <c r="A79" s="1">
         <v>42592</v>
       </c>
@@ -3705,7 +3742,7 @@
         <v>0.24778024125281486</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11">
       <c r="A80" s="1">
         <v>42599</v>
       </c>
@@ -3741,7 +3778,7 @@
         <v>0.33432095243321536</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11">
       <c r="A81" s="1">
         <v>42606</v>
       </c>
@@ -3777,7 +3814,7 @@
         <v>0.24022272444013409</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11">
       <c r="A82" s="1">
         <v>42613</v>
       </c>
@@ -3813,7 +3850,7 @@
         <v>-6.5824355255362066E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11">
       <c r="A83" s="1">
         <v>42620</v>
       </c>
@@ -3849,7 +3886,7 @@
         <v>-3.1927313369297716E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11">
       <c r="A84" s="1">
         <v>42627</v>
       </c>
@@ -3885,7 +3922,7 @@
         <v>-5.518900350458994E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11">
       <c r="A85" s="1">
         <v>42634</v>
       </c>
@@ -3921,7 +3958,7 @@
         <v>-8.8688420634698006E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11">
       <c r="A86" s="1">
         <v>42641</v>
       </c>
@@ -3957,7 +3994,7 @@
         <v>-0.11148311246047055</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11">
       <c r="A87" s="1">
         <v>42648</v>
       </c>
@@ -3993,7 +4030,7 @@
         <v>-0.12229427820170474</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11">
       <c r="A88" s="1">
         <v>42655</v>
       </c>
@@ -4029,7 +4066,7 @@
         <v>-1.4508147157560936E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11">
       <c r="A89" s="1">
         <v>42662</v>
       </c>
@@ -4065,7 +4102,7 @@
         <v>0.29386385191640402</v>
       </c>
     </row>
-    <row r="90" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" s="3" customFormat="1">
       <c r="A90" s="2">
         <v>42669</v>
       </c>
@@ -4103,8 +4140,9 @@
       <c r="J90" s="5">
         <v>-2.2499999999999999E-2</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K90" s="5"/>
+    </row>
+    <row r="91" spans="1:11">
       <c r="A91" s="1">
         <v>42676</v>
       </c>
@@ -4140,7 +4178,7 @@
         <v>0.5616423353433837</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11">
       <c r="A92" s="1">
         <v>42683</v>
       </c>
@@ -4176,7 +4214,7 @@
         <v>0.64870524524487205</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11">
       <c r="A93" s="1">
         <v>42690</v>
       </c>
@@ -4212,7 +4250,7 @@
         <v>0.5781988693510195</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11">
       <c r="A94" s="1">
         <v>42697</v>
       </c>
@@ -4248,7 +4286,7 @@
         <v>0.5692196786980358</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11">
       <c r="A95" s="1">
         <v>42704</v>
       </c>
@@ -4284,7 +4322,7 @@
         <v>0.63758547590622316</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11">
       <c r="A96" s="1">
         <v>42711</v>
       </c>
@@ -4320,7 +4358,7 @@
         <v>0.54791842450296824</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11">
       <c r="A97" s="1">
         <v>42718</v>
       </c>
@@ -4356,7 +4394,7 @@
         <v>0.35379656197946946</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11">
       <c r="A98" s="1">
         <v>42725</v>
       </c>
@@ -4376,7 +4414,7 @@
         <v>-0.288586302947476</v>
       </c>
       <c r="F98">
-        <f t="shared" ref="F98:F112" si="20">B98-$L$1</f>
+        <f t="shared" ref="F98:F112" si="20">B98-$M$1</f>
         <v>-0.476819517945204</v>
       </c>
       <c r="G98">
@@ -4392,7 +4430,7 @@
         <v>0.20037079705252397</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11">
       <c r="A99" s="1">
         <v>42732</v>
       </c>
@@ -4416,7 +4454,7 @@
         <v>-0.48913547050574607</v>
       </c>
       <c r="G99">
-        <f t="shared" ref="G99:G112" si="21">C99-$L$1</f>
+        <f t="shared" ref="G99:G112" si="21">C99-$M$1</f>
         <v>-0.48297749422547503</v>
       </c>
       <c r="H99">
@@ -4428,7 +4466,7 @@
         <v>3.6726672449953979E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11">
       <c r="A100" s="1">
         <v>42739</v>
       </c>
@@ -4464,7 +4502,7 @@
         <v>2.2315700987434739E-3</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11">
       <c r="A101" s="1">
         <v>42746</v>
       </c>
@@ -4492,7 +4530,7 @@
         <v>0.30365477076278646</v>
       </c>
       <c r="H101">
-        <f t="shared" ref="H101:H112" si="23">D101-$L$1</f>
+        <f t="shared" ref="H101:H112" si="23">D101-$M$1</f>
         <v>-8.9661361731344369E-2</v>
       </c>
       <c r="I101">
@@ -4500,7 +4538,7 @@
         <v>3.6977074726754433E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11">
       <c r="A102" s="1">
         <v>42753</v>
       </c>
@@ -4536,7 +4574,7 @@
         <v>-0.14601411442194062</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11">
       <c r="A103" s="1">
         <v>42760</v>
       </c>
@@ -4572,7 +4610,7 @@
         <v>-0.3407522643742224</v>
       </c>
     </row>
-    <row r="104" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" s="3" customFormat="1">
       <c r="A104" s="2">
         <v>42767</v>
       </c>
@@ -4610,8 +4648,9 @@
       <c r="J104" s="5">
         <v>6.0999999999999999E-2</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K104" s="5"/>
+    </row>
+    <row r="105" spans="1:11">
       <c r="A105" s="1">
         <v>42774</v>
       </c>
@@ -4643,11 +4682,11 @@
         <v>-1.6539819675451095E-2</v>
       </c>
       <c r="I105">
-        <f t="shared" ref="I105:I112" si="25">E105-$L$1</f>
+        <f t="shared" ref="I105:I112" si="25">E105-$M$1</f>
         <v>-5.3100590703397732E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11">
       <c r="A106" s="1">
         <v>42781</v>
       </c>
@@ -4683,7 +4722,7 @@
         <v>6.3721113362584791E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11">
       <c r="A107" s="1">
         <v>42788</v>
       </c>
@@ -4719,7 +4758,7 @@
         <v>0.22048989719614326</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11">
       <c r="A108" s="1">
         <v>42795</v>
       </c>
@@ -4755,7 +4794,7 @@
         <v>0.21069206307358163</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11">
       <c r="A109" s="1">
         <v>42802</v>
       </c>
@@ -4791,7 +4830,7 @@
         <v>0.25847613230566996</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11">
       <c r="A110" s="1">
         <v>42809</v>
       </c>
@@ -4827,7 +4866,7 @@
         <v>0.52957099843039945</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11">
       <c r="A111" s="1">
         <v>42816</v>
       </c>
@@ -4863,7 +4902,7 @@
         <v>0.723683471713503</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11">
       <c r="A112" s="1">
         <v>42823</v>
       </c>
@@ -4901,6 +4940,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4912,21 +4957,20 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.54296875" customWidth="1"/>
-    <col min="2" max="2" width="7.54296875" customWidth="1"/>
-    <col min="3" max="3" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12">
       <c r="A1" t="str">
         <f>apple_averages!A1</f>
         <v>Week</v>
@@ -4968,15 +5012,15 @@
         <v>PxCh</v>
       </c>
       <c r="K1" t="str">
-        <f>apple_averages!K1</f>
+        <f>apple_averages!L1</f>
         <v>Base Sentiment</v>
       </c>
       <c r="L1">
-        <f>apple_averages!L1</f>
+        <f>apple_averages!M1</f>
         <v>-0.48895709999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <f>apple_averages!A12</f>
         <v>42123</v>
@@ -5018,7 +5062,7 @@
         <v>-1.5800000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <f>apple_averages!A24</f>
         <v>42207</v>
@@ -5060,7 +5104,7 @@
         <v>-4.2299999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <f>apple_averages!A38</f>
         <v>42305</v>
@@ -5102,7 +5146,7 @@
         <v>4.1200000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <f>apple_averages!A51</f>
         <v>42396</v>
@@ -5144,7 +5188,7 @@
         <v>-6.5699999999999995E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <f>apple_averages!A64</f>
         <v>42487</v>
@@ -5186,7 +5230,7 @@
         <v>-6.2600000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <f>apple_averages!A77</f>
         <v>42578</v>
@@ -5228,7 +5272,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <f>apple_averages!A90</f>
         <v>42669</v>
@@ -5270,7 +5314,7 @@
         <v>-2.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <f>apple_averages!A104</f>
         <v>42767</v>
@@ -5314,5 +5358,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>